<commit_message>
Missing fields of RTW
</commit_message>
<xml_diff>
--- a/RTW/Missing_Field_RTW.xlsx
+++ b/RTW/Missing_Field_RTW.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Missing fields of RTW Report</t>
   </si>
@@ -28,15 +28,6 @@
   </si>
   <si>
     <t>Note</t>
-  </si>
-  <si>
-    <t>Remuneration_Start</t>
-  </si>
-  <si>
-    <t>Remuneration_End</t>
-  </si>
-  <si>
-    <t>Measure_months</t>
   </si>
   <si>
     <t>LT</t>
@@ -297,11 +288,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -312,14 +300,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -625,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,126 +627,105 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+    </row>
+    <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" ht="255" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>14</v>
+      <c r="A10" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" ht="255" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="2"/>
+      <c r="C11" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Put some comments to each missing fields
</commit_message>
<xml_diff>
--- a/RTW/Missing_Field_RTW.xlsx
+++ b/RTW/Missing_Field_RTW.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="12435" windowHeight="9015"/>
+    <workbookView xWindow="360" yWindow="195" windowWidth="12435" windowHeight="8955"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Missing Fields" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Missing fields of RTW Report</t>
   </si>
@@ -33,9 +33,6 @@
     <t>LT</t>
   </si>
   <si>
-    <t>calculated field</t>
-  </si>
-  <si>
     <t>WGT</t>
   </si>
   <si>
@@ -86,31 +83,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> / wc_Hours &amp; wc_Minutes</t>
-    </r>
-  </si>
-  <si>
-    <t>Cert_Type</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Medical_Cert </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/ Type</t>
     </r>
   </si>
   <si>
@@ -238,13 +210,72 @@
       </rPr>
       <t>/ Cost_Code2</t>
     </r>
+  </si>
+  <si>
+    <t>Might be implemented as reference data or its own dimension</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">_ Calculate the weighted claim numbers
+_ Each claim makes a contribution to the measure or has a weight associated with it = 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Number of Working Days during the relevant Assessment Period</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Maximum number of working days in the Duration band</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Calculate the Lost Time measurement during the relevant Assessment Period (in days)</t>
+  </si>
+  <si>
+    <t>This one should be gone along with calculating LT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,6 +294,36 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -288,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -298,19 +359,28 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -318,6 +388,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0000FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -616,122 +691,121 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C6" s="10"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C7" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C8" s="10"/>
+    </row>
+    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" ht="255" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C10" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="C10:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>